<commit_message>
improve - using ROE terminology
</commit_message>
<xml_diff>
--- a/investment/investment.xlsx
+++ b/investment/investment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="损益" sheetId="1" r:id="rId1"/>
@@ -38,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>收益率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>市场</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,6 +75,10 @@
   </si>
   <si>
     <t>美股原始股账户</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资产收益率（ROE）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -155,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -178,50 +178,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -234,68 +197,62 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="7" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -605,175 +562,175 @@
     <col min="4" max="4" width="16.375" style="2" customWidth="1"/>
     <col min="5" max="5" width="13.25" style="2" customWidth="1"/>
     <col min="6" max="6" width="15.25" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="B2" s="4">
         <v>42005</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="5">
         <v>160000</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="6">
         <v>156424.13</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8">
         <f>(D2-C2)/C2</f>
         <v>-2.2349187499999972E-2</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="4"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="4"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="4"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="8">
+      <c r="A6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4">
         <v>42005</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="9">
         <v>31148.33</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="10">
         <v>31678.66</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="15">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="11">
         <f t="shared" ref="G6:G10" si="0">(D6-C6)/C6</f>
         <v>1.7025952916255801E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="4"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="15"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="4"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="15"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="4"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="15"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8">
+      <c r="A10" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4">
         <v>42005</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="12">
         <f>C6*6.2743+C2</f>
         <v>355433.96691900003</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="13">
         <f>D6*6.2743+D2</f>
         <v>355185.54643800005</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12">
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8">
         <f t="shared" si="0"/>
         <v>-6.9892161166631495E-4</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="6"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="7"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -791,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -807,269 +764,269 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="20">
+      <c r="A2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="16">
         <v>42005</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="17">
         <v>160000</v>
       </c>
-      <c r="D2" s="21">
-        <v>0</v>
-      </c>
-      <c r="E2" s="21">
-        <v>0</v>
-      </c>
-      <c r="F2" s="21">
+      <c r="D2" s="17">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17">
+        <v>0</v>
+      </c>
+      <c r="F2" s="17">
         <f>C2-D2+E2</f>
         <v>160000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20">
+      <c r="A3" s="22"/>
+      <c r="B3" s="16">
         <v>42045</v>
       </c>
-      <c r="C3" s="21">
-        <v>0</v>
-      </c>
-      <c r="D3" s="21">
-        <v>0</v>
-      </c>
-      <c r="E3" s="21">
+      <c r="C3" s="17">
+        <v>0</v>
+      </c>
+      <c r="D3" s="17">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17">
         <v>403.09</v>
       </c>
-      <c r="F3" s="21">
+      <c r="F3" s="17">
         <f>F2+C3-D3+E3</f>
         <v>160403.09</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="19"/>
-      <c r="B4" s="20">
+      <c r="A4" s="22"/>
+      <c r="B4" s="16">
         <v>42051</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="17">
         <v>31000</v>
       </c>
-      <c r="D4" s="21">
-        <v>0</v>
-      </c>
-      <c r="E4" s="21">
-        <v>0</v>
-      </c>
-      <c r="F4" s="21">
+      <c r="D4" s="17">
+        <v>0</v>
+      </c>
+      <c r="E4" s="17">
+        <v>0</v>
+      </c>
+      <c r="F4" s="17">
         <f>F3+C4-D4+E4</f>
         <v>191403.09</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20">
+      <c r="A5" s="22"/>
+      <c r="B5" s="16">
         <v>42063</v>
       </c>
-      <c r="C5" s="21">
-        <v>0</v>
-      </c>
-      <c r="D5" s="21">
-        <v>0</v>
-      </c>
-      <c r="E5" s="21">
+      <c r="C5" s="17">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17">
         <v>59.61</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="17">
         <f>F4+C5-D5+E5</f>
         <v>191462.69999999998</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="19"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="19"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="19"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="19"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="20">
+      <c r="A11" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="16">
         <v>41639</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="20">
         <v>13684</v>
       </c>
-      <c r="D11" s="24">
-        <v>0</v>
-      </c>
-      <c r="E11" s="24">
-        <v>0</v>
-      </c>
-      <c r="F11" s="24">
+      <c r="D11" s="20">
+        <v>0</v>
+      </c>
+      <c r="E11" s="20">
+        <v>0</v>
+      </c>
+      <c r="F11" s="20">
         <v>13684</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20">
+      <c r="A12" s="22"/>
+      <c r="B12" s="16">
         <v>41992</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="20">
         <v>3071.25</v>
       </c>
-      <c r="D12" s="24">
-        <v>0</v>
-      </c>
-      <c r="E12" s="24">
-        <v>0</v>
-      </c>
-      <c r="F12" s="24">
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20">
+        <v>0</v>
+      </c>
+      <c r="F12" s="20">
         <f>F11+C12-D12+E12</f>
         <v>16755.25</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20">
+      <c r="A13" s="22"/>
+      <c r="B13" s="16">
         <v>42004</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="20">
         <v>14393.08</v>
       </c>
-      <c r="D13" s="24">
-        <v>0</v>
-      </c>
-      <c r="E13" s="24">
-        <v>0</v>
-      </c>
-      <c r="F13" s="24">
+      <c r="D13" s="20">
+        <v>0</v>
+      </c>
+      <c r="E13" s="20">
+        <v>0</v>
+      </c>
+      <c r="F13" s="20">
         <f>F12+C13-D13+E13</f>
         <v>31148.33</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="18"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>